<commit_message>
update mapping schemes for Ecuador and Argentina
</commit_message>
<xml_diff>
--- a/South_America/_Metadata/Mapping_Schemes/Mapping_Argentina_Res.xlsx
+++ b/South_America/_Metadata/Mapping_Schemes/Mapping_Argentina_Res.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria Camila\Documents\Git_repositories\GEM\WIP\south_america\data\processed\residential\0_censos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria Camila\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1D2406-39CE-4A4D-A922-52ADEFA8DCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE953B6F-FB4F-4CB1-B0D8-989D265C2078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="679" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping_Urban" sheetId="10" r:id="rId1"/>
@@ -1546,12 +1546,12 @@
   </sheetPr>
   <dimension ref="A1:Z89"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+    <sheetView view="pageBreakPreview" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H7" sqref="H7"/>
       <selection pane="topRight" activeCell="H7" sqref="H7"/>
       <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15"/>
@@ -2264,11 +2264,11 @@
   </sheetPr>
   <dimension ref="A1:Z65"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15"/>
@@ -2348,7 +2348,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>58</v>
@@ -2405,7 +2405,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Update Adm1 South_America summaries
</commit_message>
<xml_diff>
--- a/South_America/_Metadata/Mapping_Schemes/Mapping_Argentina_Res.xlsx
+++ b/South_America/_Metadata/Mapping_Schemes/Mapping_Argentina_Res.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria Camila\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria Camila\Documents\Git_repositories\GEM\WIP\south_america\data\processed\residential\0_censos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE953B6F-FB4F-4CB1-B0D8-989D265C2078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1D2406-39CE-4A4D-A922-52ADEFA8DCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="679" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping_Urban" sheetId="10" r:id="rId1"/>
@@ -1546,12 +1546,12 @@
   </sheetPr>
   <dimension ref="A1:Z89"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H7" sqref="H7"/>
       <selection pane="topRight" activeCell="H7" sqref="H7"/>
       <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15"/>
@@ -2264,11 +2264,11 @@
   </sheetPr>
   <dimension ref="A1:Z65"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView view="pageBreakPreview" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15"/>
@@ -2348,7 +2348,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>58</v>
@@ -2405,7 +2405,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>58</v>

</xml_diff>